<commit_message>
added tagconnect to bom
</commit_message>
<xml_diff>
--- a/documentation/bom-component-request.xlsx
+++ b/documentation/bom-component-request.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19095" windowHeight="12315" tabRatio="500"/>
+    <workbookView windowWidth="19095" windowHeight="12375" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Mouser" sheetId="4" r:id="rId1"/>
-    <sheet name="Farnell" sheetId="5" r:id="rId2"/>
+    <sheet name="Digikey" sheetId="5" r:id="rId2"/>
     <sheet name="HobbyKing" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="114">
   <si>
     <t>Name</t>
   </si>
@@ -319,7 +319,31 @@
     <t>Motor Field Oriented Controller, BLDC, DC Motor, PMSM, Stepper</t>
   </si>
   <si>
-    <t>https://pt.farnell.com/trinamic/tmc4671-es/motor-controller-bldc-pmsm-stepper/dp/2916492?st=TMC4671</t>
+    <t>https://www.digikey.com/products/en?keywords=TMC4671-ES</t>
+  </si>
+  <si>
+    <t>Programmer cable</t>
+  </si>
+  <si>
+    <t>TagConnect</t>
+  </si>
+  <si>
+    <t>TC2050-IDC-NL-ND</t>
+  </si>
+  <si>
+    <t>Programmers  Accessories</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/tag-connect-llc/TC2050-IDC-NL/TC2050-IDC-NL-ND/2605367</t>
+  </si>
+  <si>
+    <t>tc cable clip</t>
+  </si>
+  <si>
+    <t>TC2050-CLIP-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/tag-connect-llc/TC2050-CLIP/TC2050-CLIP-ND/2605374</t>
   </si>
   <si>
     <t>BLDC</t>
@@ -342,10 +366,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -363,34 +387,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -398,29 +406,9 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -434,7 +422,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,6 +431,13 @@
       <b/>
       <sz val="18"/>
       <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -457,38 +452,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -504,7 +483,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -516,6 +510,36 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -538,49 +562,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -592,7 +706,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -604,121 +730,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -917,6 +941,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -936,17 +975,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -977,6 +1010,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -991,165 +1033,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1201,13 +1225,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="48" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1219,7 +1246,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1240,7 +1267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1641,8 +1668,8 @@
   </sheetPr>
   <dimension ref="B1:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -1723,7 +1750,7 @@
       <c r="G4" s="13">
         <v>5</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="26" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1746,7 +1773,7 @@
       <c r="G5" s="13">
         <v>1</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="26" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1769,7 +1796,7 @@
       <c r="G6" s="13">
         <v>3</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="26" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1792,7 +1819,7 @@
       <c r="G7" s="13">
         <v>1</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="26" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1815,7 +1842,7 @@
       <c r="G8" s="13">
         <v>10</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="26" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1829,16 +1856,16 @@
       <c r="D9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="27" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="13">
-        <v>10</v>
-      </c>
-      <c r="H9" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="26" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1855,36 +1882,36 @@
       <c r="E10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="26" t="s">
+      <c r="F10" s="27" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="13">
         <v>5</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="26" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="11" ht="16" customHeight="1" spans="2:8">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="18" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="26" t="s">
+      <c r="F11" s="27" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="13">
         <v>2</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="26" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1892,7 +1919,7 @@
       <c r="B12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="20" t="s">
         <v>47</v>
       </c>
       <c r="D12" s="7" t="s">
@@ -1901,13 +1928,13 @@
       <c r="E12" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="27" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="13">
         <v>2</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="26" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1924,13 +1951,13 @@
       <c r="E13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="27" t="s">
         <v>11</v>
       </c>
       <c r="G13" s="13">
         <v>100</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="26" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1947,13 +1974,13 @@
       <c r="E14" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="27" t="s">
         <v>11</v>
       </c>
       <c r="G14" s="13">
         <v>10</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="26" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1964,168 +1991,168 @@
       <c r="C15" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="26">
+      <c r="G15" s="27">
         <v>20</v>
       </c>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="26" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" ht="16" customHeight="1" spans="2:8">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="26" t="s">
+      <c r="F16" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="27">
         <v>100</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="26" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="17" ht="16" customHeight="1" spans="2:8">
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="26" t="s">
+      <c r="F17" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="27">
         <v>100</v>
       </c>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="26" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="18" ht="16" customHeight="1" spans="2:8">
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F18" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="27">
         <v>50</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H18" s="26" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="19" ht="16" customHeight="1" spans="2:8">
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="27">
         <v>50</v>
       </c>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="26" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" ht="16" customHeight="1" spans="2:8">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="23" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="26" t="s">
+      <c r="F20" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="27">
         <v>5</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="26" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="21" ht="16" customHeight="1" spans="2:8">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="22" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="26">
+      <c r="G21" s="27">
         <v>2</v>
       </c>
-      <c r="H21" s="25" t="s">
+      <c r="H21" s="26" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="22" ht="16" customHeight="1" spans="2:8">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="19" t="s">
         <v>88</v>
       </c>
       <c r="E22" s="7" t="s">
@@ -2137,7 +2164,7 @@
       <c r="G22" s="13">
         <v>5</v>
       </c>
-      <c r="H22" s="25" t="s">
+      <c r="H22" s="26" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2154,13 +2181,13 @@
       <c r="E23" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="F23" s="27" t="s">
+      <c r="F23" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="28">
         <v>5</v>
       </c>
-      <c r="H23" s="28" t="s">
+      <c r="H23" s="29" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2168,13 +2195,13 @@
       <c r="B24" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="25" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="25" ht="16" customHeight="1"/>
     <row r="32" spans="6:6">
-      <c r="F32" s="29"/>
+      <c r="F32" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2212,8 +2239,8 @@
   </sheetPr>
   <dimension ref="B1:H26"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="12.75" outlineLevelCol="7"/>
@@ -2269,29 +2296,57 @@
         <v>11</v>
       </c>
       <c r="G3" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="14"/>
+      <c r="B4" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="14"/>
+      <c r="B5" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="7">
+        <v>1</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="6"/>
@@ -2476,7 +2531,9 @@
     <row r="26" ht="13.5"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" display="https://pt.farnell.com/trinamic/tmc4671-es/motor-controller-bldc-pmsm-stepper/dp/2916492?st=TMC4671" tooltip="https://pt.farnell.com/trinamic/tmc4671-es/motor-controller-bldc-pmsm-stepper/dp/2916492?st=TMC4671"/>
+    <hyperlink ref="H3" r:id="rId1" display="https://www.digikey.com/products/en?keywords=TMC4671-ES" tooltip="https://www.digikey.com/products/en?keywords=TMC4671-ES"/>
+    <hyperlink ref="H4" r:id="rId2" display="https://www.digikey.com/product-detail/en/tag-connect-llc/TC2050-IDC-NL/TC2050-IDC-NL-ND/2605367"/>
+    <hyperlink ref="H5" r:id="rId3" display="https://www.digikey.com/product-detail/en/tag-connect-llc/TC2050-CLIP/TC2050-CLIP-ND/2605374"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2532,16 +2589,16 @@
     </row>
     <row r="3" ht="16" customHeight="1" spans="2:8">
       <c r="B3" s="3" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>11</v>
@@ -2550,7 +2607,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:8">

</xml_diff>